<commit_message>
Review page issues fixed, and Equipments filtered with respect to plans Selected, Data Corrected in xlsx
</commit_message>
<xml_diff>
--- a/Src/VzMach/VzMach/App_Data/Data.xlsx
+++ b/Src/VzMach/VzMach/App_Data/Data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\HackMach1\Src\VzMach\VzMach\App_Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28215" windowHeight="13020"/>
+    <workbookView windowWidth="28220" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$J$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$J$68</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141">
   <si>
     <t>Zipcode</t>
   </si>
@@ -50,345 +45,378 @@
     <t>NJ</t>
   </si>
   <si>
+    <t>B0003,B0004</t>
+  </si>
+  <si>
     <t>B0013,B0032</t>
   </si>
   <si>
+    <t>B0017,B0020,B0057</t>
+  </si>
+  <si>
+    <t>C0004,C0008</t>
+  </si>
+  <si>
+    <t>76248</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>B0015,B0016</t>
+  </si>
+  <si>
+    <t>C0002,C0008</t>
+  </si>
+  <si>
+    <t>22042</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B0023,B0024 </t>
+  </si>
+  <si>
+    <t>C0001,C0008</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>B0036,B0011</t>
+  </si>
+  <si>
+    <t>89101</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>B0017,B0040</t>
+  </si>
+  <si>
+    <t>C0006,C0008</t>
+  </si>
+  <si>
+    <t>75039</t>
+  </si>
+  <si>
+    <t>B0017,B0001</t>
+  </si>
+  <si>
+    <t>BundleId</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>DAT</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>VOICE</t>
+  </si>
+  <si>
+    <t>ROUTER</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>B0001</t>
+  </si>
+  <si>
+    <t>CORE</t>
+  </si>
+  <si>
+    <t>TriplePlay</t>
+  </si>
+  <si>
+    <t>50M</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>Unlimited</t>
+  </si>
+  <si>
+    <t>DAT_TV_VOICE</t>
+  </si>
+  <si>
+    <t>B0002</t>
+  </si>
+  <si>
+    <t>Prime</t>
+  </si>
+  <si>
+    <t>B0003</t>
+  </si>
+  <si>
+    <t>Extreme</t>
+  </si>
+  <si>
+    <t>B0004</t>
+  </si>
+  <si>
+    <t>Ultimate</t>
+  </si>
+  <si>
+    <t>B0005</t>
+  </si>
+  <si>
+    <t>75M</t>
+  </si>
+  <si>
+    <t>B0006</t>
+  </si>
+  <si>
+    <t>B0007</t>
+  </si>
+  <si>
+    <t>B0008</t>
+  </si>
+  <si>
+    <t>B0009</t>
+  </si>
+  <si>
+    <t>100M</t>
+  </si>
+  <si>
+    <t>B0010</t>
+  </si>
+  <si>
+    <t>B0011</t>
+  </si>
+  <si>
+    <t>B0012</t>
+  </si>
+  <si>
+    <t>B0013</t>
+  </si>
+  <si>
+    <t>150M</t>
+  </si>
+  <si>
+    <t>B0014</t>
+  </si>
+  <si>
+    <t>B0015</t>
+  </si>
+  <si>
+    <t>B0016</t>
+  </si>
+  <si>
+    <t>B0017</t>
+  </si>
+  <si>
+    <t>1G</t>
+  </si>
+  <si>
+    <t>B0018</t>
+  </si>
+  <si>
+    <t>B0019</t>
+  </si>
+  <si>
+    <t>B0020</t>
+  </si>
+  <si>
+    <t>B0021</t>
+  </si>
+  <si>
+    <t>DoublePlay</t>
+  </si>
+  <si>
+    <t>DAT_TV</t>
+  </si>
+  <si>
+    <t>B0022</t>
+  </si>
+  <si>
+    <t>B0023</t>
+  </si>
+  <si>
+    <t>B0024</t>
+  </si>
+  <si>
+    <t>B0025</t>
+  </si>
+  <si>
+    <t>B0026</t>
+  </si>
+  <si>
+    <t>B0027</t>
+  </si>
+  <si>
+    <t>B0028</t>
+  </si>
+  <si>
+    <t>B0029</t>
+  </si>
+  <si>
+    <t>B0030</t>
+  </si>
+  <si>
+    <t>B0031</t>
+  </si>
+  <si>
+    <t>B0032</t>
+  </si>
+  <si>
+    <t>B0033</t>
+  </si>
+  <si>
+    <t>B0034</t>
+  </si>
+  <si>
+    <t>B0035</t>
+  </si>
+  <si>
+    <t>B0036</t>
+  </si>
+  <si>
+    <t>B0037</t>
+  </si>
+  <si>
+    <t>B0038</t>
+  </si>
+  <si>
+    <t>B0039</t>
+  </si>
+  <si>
+    <t>B0040</t>
+  </si>
+  <si>
+    <t>B0041</t>
+  </si>
+  <si>
+    <t>DAT_VOICE</t>
+  </si>
+  <si>
+    <t>B0045</t>
+  </si>
+  <si>
+    <t>B0049</t>
+  </si>
+  <si>
+    <t>B0053</t>
+  </si>
+  <si>
+    <t>B0057</t>
+  </si>
+  <si>
+    <t>B0061</t>
+  </si>
+  <si>
+    <t>TV_VOICE</t>
+  </si>
+  <si>
+    <t>B0062</t>
+  </si>
+  <si>
+    <t>B0063</t>
+  </si>
+  <si>
+    <t>B0064</t>
+  </si>
+  <si>
+    <t>S0001</t>
+  </si>
+  <si>
+    <t>CORE_ALONE</t>
+  </si>
+  <si>
+    <t>Fios Data</t>
+  </si>
+  <si>
+    <t>S0002</t>
+  </si>
+  <si>
+    <t>S0003</t>
+  </si>
+  <si>
+    <t>S0004</t>
+  </si>
+  <si>
+    <t>S0005</t>
+  </si>
+  <si>
+    <t>S0006</t>
+  </si>
+  <si>
+    <t>FioS TV</t>
+  </si>
+  <si>
+    <t>S0007</t>
+  </si>
+  <si>
+    <t>S0008</t>
+  </si>
+  <si>
+    <t>S0009</t>
+  </si>
+  <si>
+    <t>S0010</t>
+  </si>
+  <si>
+    <t>Fios Voice</t>
+  </si>
+  <si>
+    <t>C0001</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>1 TV+ Enhanced Recording</t>
+  </si>
+  <si>
+    <t>BHR4</t>
+  </si>
+  <si>
+    <t>REC_ROT</t>
+  </si>
+  <si>
+    <t>C0002</t>
+  </si>
+  <si>
+    <t>2 TV+ Enhanced Recording</t>
+  </si>
+  <si>
+    <t>C0003</t>
+  </si>
+  <si>
+    <t>2 TV+ Premium Recording</t>
+  </si>
+  <si>
     <t>C0004</t>
   </si>
   <si>
-    <t>76248</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>C0002</t>
-  </si>
-  <si>
-    <t>22042</t>
-  </si>
-  <si>
-    <t>VA</t>
-  </si>
-  <si>
-    <t>C0001</t>
-  </si>
-  <si>
-    <t>NY</t>
-  </si>
-  <si>
-    <t>89101</t>
-  </si>
-  <si>
-    <t>NV</t>
+    <t>BHR5</t>
+  </si>
+  <si>
+    <t>C0005</t>
   </si>
   <si>
     <t>C0006</t>
   </si>
   <si>
-    <t>75039</t>
-  </si>
-  <si>
-    <t>BundleId</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>DAT</t>
-  </si>
-  <si>
-    <t>TV</t>
-  </si>
-  <si>
-    <t>VOICE</t>
-  </si>
-  <si>
-    <t>ROUTER</t>
-  </si>
-  <si>
-    <t>Discount</t>
-  </si>
-  <si>
-    <t>Keyword</t>
-  </si>
-  <si>
-    <t>B0001</t>
-  </si>
-  <si>
-    <t>CORE</t>
-  </si>
-  <si>
-    <t>TriplePlay</t>
-  </si>
-  <si>
-    <t>50M</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>Unlimited</t>
-  </si>
-  <si>
-    <t>DAT_TV_VOICE</t>
-  </si>
-  <si>
-    <t>B0002</t>
-  </si>
-  <si>
-    <t>Prime</t>
-  </si>
-  <si>
-    <t>B0003</t>
-  </si>
-  <si>
-    <t>Extreme</t>
-  </si>
-  <si>
-    <t>B0004</t>
-  </si>
-  <si>
-    <t>Ultimate</t>
-  </si>
-  <si>
-    <t>B0005</t>
-  </si>
-  <si>
-    <t>75M</t>
-  </si>
-  <si>
-    <t>B0006</t>
-  </si>
-  <si>
-    <t>B0007</t>
-  </si>
-  <si>
-    <t>B0008</t>
-  </si>
-  <si>
-    <t>B0009</t>
-  </si>
-  <si>
-    <t>100M</t>
-  </si>
-  <si>
-    <t>B0010</t>
-  </si>
-  <si>
-    <t>B0011</t>
-  </si>
-  <si>
-    <t>B0012</t>
-  </si>
-  <si>
-    <t>B0013</t>
-  </si>
-  <si>
-    <t>150M</t>
-  </si>
-  <si>
-    <t>B0014</t>
-  </si>
-  <si>
-    <t>B0015</t>
-  </si>
-  <si>
-    <t>B0016</t>
-  </si>
-  <si>
-    <t>B0017</t>
-  </si>
-  <si>
-    <t>1G</t>
-  </si>
-  <si>
-    <t>B0018</t>
-  </si>
-  <si>
-    <t>B0019</t>
-  </si>
-  <si>
-    <t>B0020</t>
-  </si>
-  <si>
-    <t>B0021</t>
-  </si>
-  <si>
-    <t>DoublePlay</t>
-  </si>
-  <si>
-    <t>DAT_TV</t>
-  </si>
-  <si>
-    <t>B0022</t>
-  </si>
-  <si>
-    <t>B0023</t>
-  </si>
-  <si>
-    <t>B0024</t>
-  </si>
-  <si>
-    <t>B0025</t>
-  </si>
-  <si>
-    <t>B0026</t>
-  </si>
-  <si>
-    <t>B0027</t>
-  </si>
-  <si>
-    <t>B0028</t>
-  </si>
-  <si>
-    <t>B0029</t>
-  </si>
-  <si>
-    <t>B0030</t>
-  </si>
-  <si>
-    <t>B0031</t>
-  </si>
-  <si>
-    <t>B0032</t>
-  </si>
-  <si>
-    <t>B0033</t>
-  </si>
-  <si>
-    <t>B0034</t>
-  </si>
-  <si>
-    <t>B0035</t>
-  </si>
-  <si>
-    <t>B0036</t>
-  </si>
-  <si>
-    <t>B0037</t>
-  </si>
-  <si>
-    <t>B0038</t>
-  </si>
-  <si>
-    <t>B0039</t>
-  </si>
-  <si>
-    <t>B0040</t>
-  </si>
-  <si>
-    <t>B0041</t>
-  </si>
-  <si>
-    <t>DAT_VOICE</t>
-  </si>
-  <si>
-    <t>B0045</t>
-  </si>
-  <si>
-    <t>B0049</t>
-  </si>
-  <si>
-    <t>B0053</t>
-  </si>
-  <si>
-    <t>B0057</t>
-  </si>
-  <si>
-    <t>B0061</t>
-  </si>
-  <si>
-    <t>TV_VOICE</t>
-  </si>
-  <si>
-    <t>B0062</t>
-  </si>
-  <si>
-    <t>B0063</t>
-  </si>
-  <si>
-    <t>B0064</t>
-  </si>
-  <si>
-    <t>S0001</t>
-  </si>
-  <si>
-    <t>CORE_ALONE</t>
-  </si>
-  <si>
-    <t>Fios Data</t>
-  </si>
-  <si>
-    <t>S0002</t>
-  </si>
-  <si>
-    <t>S0003</t>
-  </si>
-  <si>
-    <t>S0004</t>
-  </si>
-  <si>
-    <t>S0005</t>
-  </si>
-  <si>
-    <t>S0006</t>
-  </si>
-  <si>
-    <t>FioS TV</t>
-  </si>
-  <si>
-    <t>S0007</t>
-  </si>
-  <si>
-    <t>S0008</t>
-  </si>
-  <si>
-    <t>S0009</t>
-  </si>
-  <si>
-    <t>S0010</t>
-  </si>
-  <si>
-    <t>Fios Voice</t>
-  </si>
-  <si>
-    <t>COMP</t>
-  </si>
-  <si>
-    <t>Equipment</t>
-  </si>
-  <si>
-    <t>1 TV+ Enhanced Recording</t>
-  </si>
-  <si>
-    <t>BHR4</t>
-  </si>
-  <si>
-    <t>REC_ROT</t>
-  </si>
-  <si>
-    <t>2 TV+ Enhanced Recording</t>
-  </si>
-  <si>
-    <t>C0003</t>
-  </si>
-  <si>
-    <t>2 TV+ Premium Recording</t>
-  </si>
-  <si>
-    <t>BHR5</t>
-  </si>
-  <si>
-    <t>C0005</t>
-  </si>
-  <si>
     <t>C0007</t>
   </si>
   <si>
@@ -414,33 +442,18 @@
   </si>
   <si>
     <t>C0011</t>
-  </si>
-  <si>
-    <t>B0017,B0001</t>
-  </si>
-  <si>
-    <t>B0003,B0004</t>
-  </si>
-  <si>
-    <t>B0015,B0016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B0023,B0024 </t>
-  </si>
-  <si>
-    <t>B0036,B0011</t>
-  </si>
-  <si>
-    <t>B0017,B0040</t>
-  </si>
-  <si>
-    <t>B0017,B0020,B0057</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -490,33 +503,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Comma[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
+    <cellStyle name="Currency[0]" xfId="5" builtinId="7"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -815,7 +838,6 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -848,22 +870,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42857142857143" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.57142857142857" customWidth="1"/>
+    <col min="3" max="3" width="12.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="19.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="17.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.28571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -894,56 +917,56 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>133</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -951,1710 +974,1710 @@
         <v>11385</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>135</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="7" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="24.4285714285714" customWidth="1"/>
+    <col min="7" max="8" width="9.85714285714286" customWidth="1"/>
+    <col min="9" max="9" width="8.71428571428571" customWidth="1"/>
+    <col min="10" max="10" width="14.4285714285714" customWidth="1"/>
+    <col min="11" max="11" width="15.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" hidden="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1">
         <f>(D51+D56+D60)</f>
         <v>114.98</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1">
         <f>(D51+D57+D60)</f>
         <v>124.98</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D4" s="1">
         <f>(D51+D58+D60)</f>
-        <v>129.98000000000002</v>
+        <v>129.98</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1">
         <f>(D51+D59+D60)</f>
-        <v>139.98000000000002</v>
+        <v>139.98</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1">
         <f>(D52+D60+D60)</f>
-        <v>119.99000000000001</v>
+        <v>119.99</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1">
         <f>(D52+G61+D60)</f>
-        <v>89.990000000000009</v>
+        <v>89.99</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1">
         <f>(D52+G62+D60)</f>
-        <v>89.990000000000009</v>
+        <v>89.99</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1">
         <f>(D52+G63+D60)</f>
-        <v>89.990000000000009</v>
+        <v>89.99</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1">
         <f>(D53+D56+D60)</f>
-        <v>139.97999999999999</v>
+        <v>139.98</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1">
         <f>(D53+D57+D60)</f>
-        <v>149.97999999999999</v>
+        <v>149.98</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1">
         <f>(D53+D58+D60)</f>
-        <v>154.97999999999999</v>
+        <v>154.98</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1">
         <f>(D53+D59+D60)</f>
         <v>164.98</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D14" s="1">
         <f>(D54+D56+D60)</f>
-        <v>149.97999999999999</v>
+        <v>149.98</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1">
         <f>(D54+D57+D60)</f>
-        <v>159.97999999999999</v>
+        <v>159.98</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1">
         <f>(D54+D58+D60)</f>
         <v>164.98</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1">
         <f>(D54+D59+D60)</f>
         <v>174.98</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1">
         <f>(D55+D56+D60)</f>
-        <v>214.98000000000002</v>
+        <v>214.98</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1">
         <f>(D55+D57+D60)</f>
-        <v>224.98000000000002</v>
+        <v>224.98</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D20" s="1">
         <f>(D55+D58+D60)</f>
-        <v>229.98000000000002</v>
+        <v>229.98</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1">
         <f>(D55+D59+D60)</f>
-        <v>239.98000000000002</v>
+        <v>239.98</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" hidden="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D22" s="1">
         <f>(D51+D56)</f>
         <v>84.98</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D23" s="1">
         <f>(D51+D57)</f>
         <v>94.98</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D24" s="1">
         <f>(D51+D58)</f>
         <v>99.98</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D25" s="1">
         <f>(D51+D59)</f>
         <v>109.98</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="W25" s="3"/>
     </row>
-    <row r="26" spans="1:23" hidden="1">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D26" s="1">
         <f>(D52+D56)</f>
         <v>94.98</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D27" s="1">
         <f>(D52+D57)</f>
         <v>104.98</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D28" s="1">
         <f>(D52+D58)</f>
         <v>109.98</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D29" s="1">
         <f>(D52+D59)</f>
         <v>119.98</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D30" s="1">
         <f>(D53+D56)</f>
-        <v>109.97999999999999</v>
+        <v>109.98</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D31" s="1">
         <f>(D53+D57)</f>
-        <v>119.97999999999999</v>
+        <v>119.98</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D32" s="1">
         <f>(D53+D58)</f>
-        <v>124.97999999999999</v>
+        <v>124.98</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D33" s="1">
         <f>(D53+D59)</f>
-        <v>134.97999999999999</v>
+        <v>134.98</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D34" s="1">
         <f>(D54+D56)</f>
-        <v>119.97999999999999</v>
+        <v>119.98</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D35" s="1">
         <f>(D54+D57)</f>
-        <v>129.97999999999999</v>
+        <v>129.98</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D36" s="1">
         <f>(D54+D58)</f>
-        <v>134.97999999999999</v>
+        <v>134.98</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D37" s="1">
         <f>(D54+D59)</f>
-        <v>144.97999999999999</v>
+        <v>144.98</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D38" s="1">
         <f>(D55+D56)</f>
-        <v>184.98000000000002</v>
+        <v>184.98</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D39" s="1">
         <f>(D55+D57)</f>
-        <v>194.98000000000002</v>
+        <v>194.98</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D40" s="1">
         <f>(D55+D58)</f>
-        <v>199.98000000000002</v>
+        <v>199.98</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D41" s="1">
         <f>(D55+D59)</f>
-        <v>209.98000000000002</v>
+        <v>209.98</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" hidden="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D42" s="1">
         <f>(D51+D60)</f>
-        <v>79.990000000000009</v>
+        <v>79.99</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" hidden="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D43" s="1">
         <f>(D52+D60)</f>
-        <v>89.990000000000009</v>
+        <v>89.99</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" hidden="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D44" s="1">
         <f>(D53+D60)</f>
         <v>104.99</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" hidden="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D45" s="1">
         <f>(D54+D60)</f>
         <v>114.99</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D46" s="1">
         <f>(D55+D60)</f>
         <v>179.99</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D47" s="1">
         <f>(D56+D60)</f>
-        <v>64.990000000000009</v>
+        <v>64.99</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D48" s="1">
         <f>(D57+D60)</f>
-        <v>74.990000000000009</v>
+        <v>74.99</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" hidden="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D49" s="1">
         <f>(D58+D60)</f>
-        <v>79.990000000000009</v>
+        <v>79.99</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" hidden="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D50" s="1">
         <f>(D59+D60)</f>
-        <v>89.990000000000009</v>
+        <v>89.99</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" hidden="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D51" s="1">
         <v>49.99</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" hidden="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D52" s="1">
         <v>59.99</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" hidden="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D53" s="1">
-        <v>74.989999999999995</v>
+        <v>74.99</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" hidden="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D54" s="1">
         <v>84.99</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D55" s="1">
         <v>149.99</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" hidden="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="1" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D56" s="1">
         <v>34.99</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" hidden="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D57" s="1">
         <v>44.99</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" hidden="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D58" s="1">
         <v>49.99</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" hidden="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D59" s="1">
         <v>59.99</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" hidden="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D60" s="1">
         <v>30</v>
@@ -2662,179 +2685,179 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" hidden="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="2" t="s">
-        <v>15</v>
+        <v>118</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D61" s="2">
-        <v>19.989999999999998</v>
+        <v>19.99</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" hidden="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="2" t="s">
-        <v>12</v>
+        <v>124</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D62" s="2">
         <v>29.99</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="G62" s="1"/>
       <c r="H62" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" hidden="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="2" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D63" s="2">
         <v>39.99</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="2" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" hidden="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="2" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D64" s="2">
         <v>24.99</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="I64" s="1"/>
       <c r="J64" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" hidden="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="D65" s="2">
         <v>34.99</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" hidden="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" s="2" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D66" s="2">
         <v>44.99</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="2" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="I66" s="1"/>
       <c r="J66" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" hidden="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D67" s="2">
         <v>9.99</v>
@@ -2843,22 +2866,22 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="I67" s="1"/>
       <c r="J67" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" hidden="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" s="2" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D68" s="2">
         <v>14.99</v>
@@ -2867,101 +2890,96 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="I68" s="1"/>
       <c r="J68" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" hidden="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" s="2" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="D69" s="2">
         <v>10</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" hidden="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="2" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="D70" s="2">
         <v>20</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" s="2"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" hidden="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" s="2" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="D71" s="2">
         <v>30</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="2" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="G71" s="1"/>
       <c r="H71" s="2"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J71">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="1G"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <autoFilter ref="A1:J68"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2970,7 +2988,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>